<commit_message>
Header updates for summer uploads
</commit_message>
<xml_diff>
--- a/api/src/test/resources/summer-reporting-header-blank.xlsx
+++ b/api/src/test/resources/summer-reporting-header-blank.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F6F97-1708-42F2-B504-00ADEFDBB1F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E205DA-C602-7341-99DE-446B1A3F1976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4320" yWindow="2190" windowWidth="21600" windowHeight="11295" xr2:uid="{9568818F-0947-4E3C-A15C-8486CBB48021}"/>
+    <workbookView xWindow="4320" yWindow="2200" windowWidth="21600" windowHeight="11300" xr2:uid="{9568818F-0947-4E3C-A15C-8486CBB48021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,6 @@
     <t>Legal Surname</t>
   </si>
   <si>
-    <t>Legal Given First Name</t>
-  </si>
-  <si>
-    <t>Course</t>
-  </si>
-  <si>
     <t>Session Date</t>
   </si>
   <si>
@@ -66,17 +60,22 @@
     <t>Final Letter Grade</t>
   </si>
   <si>
-    <t>Number of Credits</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
-    <t>Final %</t>
-  </si>
-  <si>
-    <t>Birthdate
-yyyymmdd</t>
+    <t>Legal Given Name</t>
+  </si>
+  <si>
+    <t>Birthdate</t>
+  </si>
+  <si>
+    <t>Ministry Course Code and Level</t>
+  </si>
+  <si>
+    <t>Final Percent</t>
+  </si>
+  <si>
+    <t>Credits</t>
   </si>
 </sst>
 </file>
@@ -457,22 +456,22 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="H1" sqref="H1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="17.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="12.85546875" style="1" customWidth="1"/>
-    <col min="8" max="9" width="8.42578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="17.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="8.5" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -481,52 +480,52 @@
         <v>1</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>15</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3">
         <v>123456789</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F2" s="3">
         <v>20030516</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H2" s="3">
         <v>202408</v>
@@ -535,33 +534,33 @@
         <v>72</v>
       </c>
       <c r="J2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K2" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>123456799</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F3" s="3">
         <v>20030516</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H3" s="3">
         <v>202408</v>
@@ -570,33 +569,33 @@
         <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K3" s="3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>123456788</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F4" s="3">
         <v>20030516</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H4" s="3">
         <v>202408</v>
@@ -605,7 +604,7 @@
         <v>72</v>
       </c>
       <c r="J4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K4" s="3">
         <v>4</v>

</xml_diff>